<commit_message>
Added screenshots for tc75
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_System_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_System_JS.xlsx
@@ -583,6 +583,17 @@
 };</t>
   </si>
   <si>
+    <t>Change Start page</t>
+  </si>
+  <si>
+    <t>wait(3);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\ComplianceTest_JS\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
+ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="0"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
     <t>wait(3);
 validate1;
 link_Click(system_test_link);
@@ -593,19 +604,8 @@
 ClickRunTest(runtest_bottom_xpath);
 wait(10);
 validate4;
-CheckUITextContains(https://www.google.co.in/_wants_to_know_your_location);
+CheckUITextContains(https://www.google.co.in);
 press_Key(Back);</t>
-  </si>
-  <si>
-    <t>Change Start page</t>
-  </si>
-  <si>
-    <t>wait(3);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
-ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\ComplianceTest_JS\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
-ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="0"/&gt;);
-PushConfigxml;</t>
   </si>
 </sst>
 </file>
@@ -1085,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1147,13 +1147,13 @@
         <v>49</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2" t="s">
@@ -1369,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>59</v>

</xml_diff>